<commit_message>
Fixed some layout problems.
</commit_message>
<xml_diff>
--- a/docs/distributionplan.xlsx
+++ b/docs/distributionplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AC829A-3BB6-41B9-BE92-A2006E87F405}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C371DA9B-C299-4646-B358-B89EEEA148BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>André Arguello</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>Testplan</t>
+  </si>
+  <si>
+    <t>30min</t>
   </si>
 </sst>
 </file>
@@ -160,9 +166,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -172,6 +175,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -179,9 +188,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -480,381 +486,372 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="3" t="s">
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="5"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="5"/>
+      <c r="A2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="4"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="5"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="5"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="4"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="4"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="5"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="5"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="4"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="5"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="5"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="4"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="4"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="5"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="5"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="4"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="4"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="5"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="5"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="4"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="4"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="5"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="5"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="4"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="4"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="5"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="5"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="4"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="4"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="5"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="5"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="4"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="4"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="5"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="5"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="4"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="4"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="5"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="5"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="4"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="4"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="5"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="5"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="4"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="4"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="5"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="5"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="4"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="4"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="5"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="5"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="4"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="4"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="5"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="5"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="4"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="4"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="5"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="5"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="4"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="4"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="5"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="5"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="4"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="4"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="5"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="5"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="4"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="K1:P1"/>
-    <mergeCell ref="K6:P6"/>
-    <mergeCell ref="K2:P2"/>
-    <mergeCell ref="K3:P3"/>
-    <mergeCell ref="K4:P4"/>
-    <mergeCell ref="K5:P5"/>
-    <mergeCell ref="K18:P18"/>
-    <mergeCell ref="K19:P19"/>
-    <mergeCell ref="K12:P12"/>
-    <mergeCell ref="K13:P13"/>
-    <mergeCell ref="K14:P14"/>
-    <mergeCell ref="K15:P15"/>
-    <mergeCell ref="K16:P16"/>
-    <mergeCell ref="K17:P17"/>
-    <mergeCell ref="K7:P7"/>
-    <mergeCell ref="K8:P8"/>
-    <mergeCell ref="K9:P9"/>
-    <mergeCell ref="K10:P10"/>
-    <mergeCell ref="K11:P11"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A19:F19"/>
@@ -864,15 +861,28 @@
     <mergeCell ref="A14:F14"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A16:F16"/>
+    <mergeCell ref="K7:P7"/>
+    <mergeCell ref="K8:P8"/>
+    <mergeCell ref="K9:P9"/>
+    <mergeCell ref="K10:P10"/>
+    <mergeCell ref="K11:P11"/>
+    <mergeCell ref="K18:P18"/>
+    <mergeCell ref="K19:P19"/>
+    <mergeCell ref="K12:P12"/>
+    <mergeCell ref="K13:P13"/>
+    <mergeCell ref="K14:P14"/>
+    <mergeCell ref="K15:P15"/>
+    <mergeCell ref="K16:P16"/>
+    <mergeCell ref="K17:P17"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="K1:P1"/>
+    <mergeCell ref="K6:P6"/>
+    <mergeCell ref="K2:P2"/>
+    <mergeCell ref="K3:P3"/>
+    <mergeCell ref="K4:P4"/>
+    <mergeCell ref="K5:P5"/>
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>